<commit_message>
Changes to the input Excel file, .Rmd file and output scripts to change wording from `uptake` to `coverage`.
</commit_message>
<xml_diff>
--- a/data/config_inputs/lhc_config_inputs_v4_test.xlsx
+++ b/data/config_inputs/lhc_config_inputs_v4_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/andy_wilson_mlcsu_nhs_uk/Documents/Git/LHC_2/data/config_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/elliot_royle_mlcsu_nhs_uk/Documents/Git/Lung Health Checks/data/config_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="8_{3271BCB1-8B6F-41E3-BF9C-C1274E8B6C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC1B0B03-294D-4552-977D-700B0B3C1A92}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{3271BCB1-8B6F-41E3-BF9C-C1274E8B6C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF59C6BB-04C0-4AE1-8DE0-9B963B95CD1B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="15" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="16200" activeTab="1" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
   </bookViews>
   <sheets>
     <sheet name="frontpage" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>uptake_rate</t>
   </si>
   <si>
-    <t>Planned rate of uptake of lung health checks</t>
-  </si>
-  <si>
     <t>lhc_dna_rate</t>
   </si>
   <si>
@@ -935,6 +932,9 @@
   </si>
   <si>
     <t>Percentage of Patients with Suspicious Breast Lesion</t>
+  </si>
+  <si>
+    <t>Planned rate of coverage of lung health checks</t>
   </si>
 </sst>
 </file>
@@ -1542,124 +1542,124 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="107.54296875" customWidth="1"/>
+    <col min="2" max="2" width="107.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:2" s="7" customFormat="1" ht="29.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:2" s="7" customFormat="1" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="126" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B6" s="14"/>
-    </row>
-    <row r="7" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B7" s="12" t="s">
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="105" x14ac:dyDescent="0.35">
-      <c r="B8" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-    </row>
-    <row r="10" spans="2:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="B11" s="17" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B12" s="14"/>
-    </row>
-    <row r="13" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B13" s="12" t="s">
+    <row r="14" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B14" s="14" t="s">
+    <row r="15" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B15" s="16" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B16" s="8" t="s">
+    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B17" s="16" t="s">
+    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B18" s="16" t="s">
+    <row r="19" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B19" s="16" t="s">
+    <row r="20" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B20" s="16" t="s">
+    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B21" s="16" t="s">
+    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B22" s="16" t="s">
+    <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B23" s="16" t="s">
+    <row r="24" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B24" s="16" t="s">
+    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="15" x14ac:dyDescent="0.4">
-      <c r="B25" s="16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B26" s="14"/>
     </row>
-    <row r="27" spans="2:2" ht="15" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:2" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B27" s="12"/>
     </row>
   </sheetData>
@@ -1693,14 +1693,14 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1711,27 +1711,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -1752,12 +1752,12 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -1778,12 +1778,12 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -1804,12 +1804,12 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -1830,12 +1830,12 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -1856,12 +1856,12 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -1882,12 +1882,12 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -1908,12 +1908,12 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -1934,12 +1934,12 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -1960,12 +1960,12 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -1986,12 +1986,12 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -2012,12 +2012,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -2038,12 +2038,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -2064,12 +2064,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -2090,12 +2090,12 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -2116,12 +2116,12 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -2142,12 +2142,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -2168,12 +2168,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -2194,12 +2194,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
@@ -2220,12 +2220,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -2246,12 +2246,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -2296,15 +2296,15 @@
       <selection activeCell="E1" sqref="E1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2315,27 +2315,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -2356,12 +2356,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -2382,12 +2382,12 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -2408,12 +2408,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -2434,12 +2434,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -2460,12 +2460,12 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -2508,14 +2508,14 @@
       <selection activeCell="E3" sqref="E3:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2526,27 +2526,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -2567,12 +2567,12 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -2593,12 +2593,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -2619,12 +2619,12 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -2645,12 +2645,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -2671,12 +2671,12 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -2697,12 +2697,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -2723,12 +2723,12 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -2749,12 +2749,12 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -2775,12 +2775,12 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -2801,12 +2801,12 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -2827,12 +2827,12 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -2853,12 +2853,12 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -2879,12 +2879,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -2933,14 +2933,14 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2951,27 +2951,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -2992,12 +2992,12 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -3018,12 +3018,12 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -3044,12 +3044,12 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -3070,12 +3070,12 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -3096,12 +3096,12 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -3122,12 +3122,12 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -3148,12 +3148,12 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -3174,12 +3174,12 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -3200,12 +3200,12 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -3226,12 +3226,12 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -3252,12 +3252,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -3278,12 +3278,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -3304,12 +3304,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -3330,12 +3330,12 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -3356,12 +3356,12 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -3382,12 +3382,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -3408,12 +3408,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -3434,12 +3434,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
@@ -3460,12 +3460,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -3486,12 +3486,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -3536,15 +3536,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -3555,27 +3555,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -3596,12 +3596,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -3622,12 +3622,12 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -3648,12 +3648,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -3674,12 +3674,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -3700,12 +3700,12 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -3748,14 +3748,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -3766,27 +3766,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -3807,12 +3807,12 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -3833,12 +3833,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -3859,12 +3859,12 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -3885,12 +3885,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -3911,12 +3911,12 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -3937,12 +3937,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -3963,12 +3963,12 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -3989,12 +3989,12 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -4015,12 +4015,12 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -4041,12 +4041,12 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -4067,12 +4067,12 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -4093,12 +4093,12 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -4119,12 +4119,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -4169,18 +4169,18 @@
   </sheetPr>
   <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -4191,27 +4191,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -4232,12 +4232,12 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -4258,12 +4258,12 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -4284,12 +4284,12 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -4310,12 +4310,12 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -4336,12 +4336,12 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -4362,12 +4362,12 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -4388,12 +4388,12 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -4414,12 +4414,12 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -4440,12 +4440,12 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -4466,12 +4466,12 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -4492,12 +4492,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -4518,12 +4518,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -4544,12 +4544,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -4570,12 +4570,12 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -4596,12 +4596,12 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -4622,12 +4622,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -4648,12 +4648,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -4674,12 +4674,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
@@ -4700,12 +4700,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -4726,12 +4726,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -4772,18 +4772,18 @@
   </sheetPr>
   <dimension ref="B2:I8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4794,22 +4794,22 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4827,12 +4827,12 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -4853,12 +4853,12 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -4879,12 +4879,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>282</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -4905,12 +4905,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -4931,12 +4931,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -4958,7 +4958,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="VNy1VN3E9GnRdEQ2CWYZwYFWV/WLZ4BtdU7FkWVdrOVai6Eg3grmNxFFLJnmEtcihiKX1BawOyvKEl+5UhdVww==" saltValue="NBDo4+0TRCkYScKBna7NEg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="XdPK3jtUm4joHbEGrPc7nfU/0i/7F+/WalE3kPDHW1B2skAbsaX4z3sS/laQF+5BaotsDgXi4ywGX6xWD8e+eQ==" saltValue="YF2Jlfd3/pqvBdxHJtZZpg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:I8" xr:uid="{B0663B90-5FD1-472C-A49F-3D35F7B34ED7}">
@@ -4984,14 +4984,14 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -5002,27 +5002,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -5043,12 +5043,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -5069,12 +5069,12 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -5095,12 +5095,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -5121,12 +5121,12 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -5171,14 +5171,14 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -5189,27 +5189,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -5230,12 +5230,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -5256,12 +5256,12 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -5282,12 +5282,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -5308,12 +5308,12 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -5356,15 +5356,15 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -5375,27 +5375,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -5416,12 +5416,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -5442,12 +5442,12 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -5468,12 +5468,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -5494,12 +5494,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -5520,12 +5520,12 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -5568,14 +5568,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -5586,27 +5586,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -5627,12 +5627,12 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -5653,12 +5653,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -5679,12 +5679,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -5705,12 +5705,12 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -5731,12 +5731,12 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -5757,12 +5757,12 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -5783,12 +5783,12 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -5809,12 +5809,12 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -5835,12 +5835,12 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -5861,12 +5861,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -5916,14 +5916,14 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -5934,27 +5934,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -5975,12 +5975,12 @@
         <v>0.64589574595566202</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -6001,12 +6001,12 @@
         <v>0.18454164170161771</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -6027,12 +6027,12 @@
         <v>2.6363091671659671E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -6053,12 +6053,12 @@
         <v>2.3966446974236066E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -6079,12 +6079,12 @@
         <v>2.0371479928100657E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -6105,12 +6105,12 @@
         <v>1.6776512881965248E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -6131,12 +6131,12 @@
         <v>1.4379868184541639E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -6157,12 +6157,12 @@
         <v>1.0784901138406229E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -6183,12 +6183,12 @@
         <v>9.5865787896944263E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -6209,12 +6209,12 @@
         <v>8.3882564409826239E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -6235,12 +6235,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -6261,12 +6261,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -6287,12 +6287,12 @@
         <v>7.1899340922708197E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -6313,12 +6313,12 @@
         <v>4.7932893948472131E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -6339,12 +6339,12 @@
         <v>3.5949670461354099E-3</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -6365,12 +6365,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -6391,12 +6391,12 @@
         <v>2.3966446974236066E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -6417,12 +6417,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
@@ -6443,12 +6443,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -6469,12 +6469,12 @@
         <v>1.1983223487118033E-3</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -6519,15 +6519,15 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
@@ -6538,27 +6538,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -6579,12 +6579,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -6605,12 +6605,12 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -6631,12 +6631,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -6657,12 +6657,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -6683,12 +6683,12 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -6731,14 +6731,14 @@
       <selection activeCell="E3" sqref="E3:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -6749,27 +6749,27 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -6790,12 +6790,12 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -6816,12 +6816,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -6842,12 +6842,12 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -6868,12 +6868,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -6894,12 +6894,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -6920,12 +6920,12 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -6946,12 +6946,12 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -6972,12 +6972,12 @@
         <v>0.122</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -6998,12 +6998,12 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -7024,12 +7024,12 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -7050,12 +7050,12 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -7076,12 +7076,12 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>

</xml_diff>